<commit_message>
Add tabs and sorting to effect panel
</commit_message>
<xml_diff>
--- a/data/obsm_effs.xlsx
+++ b/data/obsm_effs.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fgary\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frank\PycharmProjects\OBSM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E90D3A1-09B5-4178-B1E9-629584E68F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{DA81CB50-6083-4A37-B02F-E27494894B05}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="30930" windowHeight="16770"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$109</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$109</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="236">
   <si>
     <t>Base Cost</t>
   </si>
@@ -720,13 +719,40 @@
   </si>
   <si>
     <t>Weakness to Shock</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>Debuff</t>
+  </si>
+  <si>
+    <t>Damage</t>
+  </si>
+  <si>
+    <t>Bound</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>Utility</t>
+  </si>
+  <si>
+    <t>Healing</t>
+  </si>
+  <si>
+    <t>Buff</t>
+  </si>
+  <si>
+    <t>Summon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1090,23 +1116,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{243C1198-9050-4D31-9385-CFB2A1D9CA84}">
-  <dimension ref="A1:E109"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="I81" sqref="I81"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="143.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="143.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>113</v>
       </c>
@@ -1120,10 +1147,13 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
+        <v>227</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>120</v>
       </c>
@@ -1137,10 +1167,13 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
+        <v>228</v>
+      </c>
+      <c r="F2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>121</v>
       </c>
@@ -1154,10 +1187,13 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
+        <v>228</v>
+      </c>
+      <c r="F3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>122</v>
       </c>
@@ -1171,10 +1207,13 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
+        <v>229</v>
+      </c>
+      <c r="F4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>123</v>
       </c>
@@ -1188,10 +1227,13 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
+        <v>228</v>
+      </c>
+      <c r="F5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>124</v>
       </c>
@@ -1205,10 +1247,13 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
+        <v>228</v>
+      </c>
+      <c r="F6" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>125</v>
       </c>
@@ -1222,10 +1267,13 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
+        <v>230</v>
+      </c>
+      <c r="F7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>126</v>
       </c>
@@ -1239,10 +1287,13 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
+        <v>230</v>
+      </c>
+      <c r="F8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>127</v>
       </c>
@@ -1256,10 +1307,13 @@
         <v>0</v>
       </c>
       <c r="E9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>128</v>
       </c>
@@ -1273,10 +1327,13 @@
         <v>0</v>
       </c>
       <c r="E10" t="s">
+        <v>230</v>
+      </c>
+      <c r="F10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>129</v>
       </c>
@@ -1290,10 +1347,13 @@
         <v>0</v>
       </c>
       <c r="E11" t="s">
+        <v>230</v>
+      </c>
+      <c r="F11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>130</v>
       </c>
@@ -1307,10 +1367,13 @@
         <v>0</v>
       </c>
       <c r="E12" t="s">
+        <v>230</v>
+      </c>
+      <c r="F12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>131</v>
       </c>
@@ -1324,10 +1387,13 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
+        <v>230</v>
+      </c>
+      <c r="F13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>132</v>
       </c>
@@ -1341,10 +1407,13 @@
         <v>0</v>
       </c>
       <c r="E14" t="s">
+        <v>230</v>
+      </c>
+      <c r="F14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>133</v>
       </c>
@@ -1358,10 +1427,13 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
+        <v>230</v>
+      </c>
+      <c r="F15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>134</v>
       </c>
@@ -1375,10 +1447,13 @@
         <v>0</v>
       </c>
       <c r="E16" t="s">
+        <v>230</v>
+      </c>
+      <c r="F16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>135</v>
       </c>
@@ -1392,10 +1467,13 @@
         <v>0</v>
       </c>
       <c r="E17" t="s">
+        <v>230</v>
+      </c>
+      <c r="F17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>136</v>
       </c>
@@ -1409,10 +1487,13 @@
         <v>0</v>
       </c>
       <c r="E18" t="s">
+        <v>228</v>
+      </c>
+      <c r="F18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>137</v>
       </c>
@@ -1426,10 +1507,13 @@
         <v>0</v>
       </c>
       <c r="E19" t="s">
+        <v>231</v>
+      </c>
+      <c r="F19" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>138</v>
       </c>
@@ -1443,10 +1527,13 @@
         <v>65</v>
       </c>
       <c r="E20" t="s">
+        <v>232</v>
+      </c>
+      <c r="F20" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>139</v>
       </c>
@@ -1460,10 +1547,13 @@
         <v>0</v>
       </c>
       <c r="E21" t="s">
+        <v>232</v>
+      </c>
+      <c r="F21" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>140</v>
       </c>
@@ -1477,10 +1567,13 @@
         <v>0</v>
       </c>
       <c r="E22" t="s">
+        <v>231</v>
+      </c>
+      <c r="F22" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>141</v>
       </c>
@@ -1494,10 +1587,13 @@
         <v>0</v>
       </c>
       <c r="E23" t="s">
+        <v>231</v>
+      </c>
+      <c r="F23" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>142</v>
       </c>
@@ -1511,10 +1607,13 @@
         <v>0</v>
       </c>
       <c r="E24" t="s">
+        <v>233</v>
+      </c>
+      <c r="F24" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>143</v>
       </c>
@@ -1528,10 +1627,13 @@
         <v>0</v>
       </c>
       <c r="E25" t="s">
+        <v>233</v>
+      </c>
+      <c r="F25" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>144</v>
       </c>
@@ -1545,10 +1647,13 @@
         <v>0</v>
       </c>
       <c r="E26" t="s">
+        <v>233</v>
+      </c>
+      <c r="F26" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>145</v>
       </c>
@@ -1562,10 +1667,13 @@
         <v>0</v>
       </c>
       <c r="E27" t="s">
+        <v>228</v>
+      </c>
+      <c r="F27" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>146</v>
       </c>
@@ -1579,10 +1687,13 @@
         <v>0</v>
       </c>
       <c r="E28" t="s">
+        <v>228</v>
+      </c>
+      <c r="F28" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>147</v>
       </c>
@@ -1596,10 +1707,13 @@
         <v>0</v>
       </c>
       <c r="E29" t="s">
+        <v>229</v>
+      </c>
+      <c r="F29" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>148</v>
       </c>
@@ -1613,10 +1727,13 @@
         <v>0</v>
       </c>
       <c r="E30" t="s">
+        <v>228</v>
+      </c>
+      <c r="F30" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>149</v>
       </c>
@@ -1630,10 +1747,13 @@
         <v>0</v>
       </c>
       <c r="E31" t="s">
+        <v>231</v>
+      </c>
+      <c r="F31" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>150</v>
       </c>
@@ -1647,10 +1767,13 @@
         <v>15</v>
       </c>
       <c r="E32" t="s">
+        <v>232</v>
+      </c>
+      <c r="F32" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>151</v>
       </c>
@@ -1664,10 +1787,13 @@
         <v>0</v>
       </c>
       <c r="E33" t="s">
+        <v>228</v>
+      </c>
+      <c r="F33" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>152</v>
       </c>
@@ -1681,10 +1807,13 @@
         <v>0</v>
       </c>
       <c r="E34" t="s">
+        <v>228</v>
+      </c>
+      <c r="F34" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>153</v>
       </c>
@@ -1698,10 +1827,13 @@
         <v>0</v>
       </c>
       <c r="E35" t="s">
+        <v>233</v>
+      </c>
+      <c r="F35" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>154</v>
       </c>
@@ -1715,10 +1847,13 @@
         <v>0</v>
       </c>
       <c r="E36" t="s">
+        <v>228</v>
+      </c>
+      <c r="F36" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>155</v>
       </c>
@@ -1732,10 +1867,13 @@
         <v>0</v>
       </c>
       <c r="E37" t="s">
+        <v>228</v>
+      </c>
+      <c r="F37" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>166</v>
       </c>
@@ -1749,10 +1887,13 @@
         <v>0</v>
       </c>
       <c r="E38" t="s">
+        <v>228</v>
+      </c>
+      <c r="F38" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>156</v>
       </c>
@@ -1766,10 +1907,13 @@
         <v>0</v>
       </c>
       <c r="E39" t="s">
+        <v>228</v>
+      </c>
+      <c r="F39" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>157</v>
       </c>
@@ -1783,10 +1927,13 @@
         <v>0</v>
       </c>
       <c r="E40" t="s">
+        <v>228</v>
+      </c>
+      <c r="F40" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>158</v>
       </c>
@@ -1800,10 +1947,13 @@
         <v>25</v>
       </c>
       <c r="E41" t="s">
+        <v>232</v>
+      </c>
+      <c r="F41" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>159</v>
       </c>
@@ -1817,10 +1967,13 @@
         <v>0</v>
       </c>
       <c r="E42" t="s">
+        <v>229</v>
+      </c>
+      <c r="F42" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6">
       <c r="A43" t="s">
         <v>160</v>
       </c>
@@ -1834,10 +1987,13 @@
         <v>100</v>
       </c>
       <c r="E43" t="s">
+        <v>234</v>
+      </c>
+      <c r="F43" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
         <v>161</v>
       </c>
@@ -1851,10 +2007,13 @@
         <v>100</v>
       </c>
       <c r="E44" t="s">
+        <v>234</v>
+      </c>
+      <c r="F44" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
         <v>162</v>
       </c>
@@ -1868,10 +2027,13 @@
         <v>25</v>
       </c>
       <c r="E45" t="s">
+        <v>234</v>
+      </c>
+      <c r="F45" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
         <v>163</v>
       </c>
@@ -1885,10 +2047,13 @@
         <v>150</v>
       </c>
       <c r="E46" t="s">
+        <v>234</v>
+      </c>
+      <c r="F46" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6">
       <c r="A47" t="s">
         <v>164</v>
       </c>
@@ -1902,10 +2067,13 @@
         <v>100</v>
       </c>
       <c r="E47" t="s">
+        <v>234</v>
+      </c>
+      <c r="F47" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6">
       <c r="A48" t="s">
         <v>167</v>
       </c>
@@ -1919,10 +2087,13 @@
         <v>100</v>
       </c>
       <c r="E48" t="s">
+        <v>234</v>
+      </c>
+      <c r="F48" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6">
       <c r="A49" t="s">
         <v>165</v>
       </c>
@@ -1936,10 +2107,13 @@
         <v>0</v>
       </c>
       <c r="E49" t="s">
+        <v>231</v>
+      </c>
+      <c r="F49" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
         <v>168</v>
       </c>
@@ -1953,10 +2127,13 @@
         <v>0</v>
       </c>
       <c r="E50" t="s">
+        <v>229</v>
+      </c>
+      <c r="F50" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6">
       <c r="A51" t="s">
         <v>169</v>
       </c>
@@ -1970,10 +2147,13 @@
         <v>100</v>
       </c>
       <c r="E51" t="s">
+        <v>234</v>
+      </c>
+      <c r="F51" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
         <v>170</v>
       </c>
@@ -1987,10 +2167,13 @@
         <v>0</v>
       </c>
       <c r="E52" t="s">
+        <v>232</v>
+      </c>
+      <c r="F52" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
         <v>171</v>
       </c>
@@ -2004,10 +2187,13 @@
         <v>12.5</v>
       </c>
       <c r="E53" t="s">
+        <v>232</v>
+      </c>
+      <c r="F53" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6">
       <c r="A54" t="s">
         <v>172</v>
       </c>
@@ -2021,10 +2207,13 @@
         <v>20</v>
       </c>
       <c r="E54" t="s">
+        <v>232</v>
+      </c>
+      <c r="F54" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6">
       <c r="A55" t="s">
         <v>173</v>
       </c>
@@ -2038,10 +2227,13 @@
         <v>0</v>
       </c>
       <c r="E55" t="s">
+        <v>232</v>
+      </c>
+      <c r="F55" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6">
       <c r="A56" t="s">
         <v>174</v>
       </c>
@@ -2055,10 +2247,13 @@
         <v>0</v>
       </c>
       <c r="E56" t="s">
+        <v>231</v>
+      </c>
+      <c r="F56" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6">
       <c r="A57" t="s">
         <v>175</v>
       </c>
@@ -2072,10 +2267,13 @@
         <v>0</v>
       </c>
       <c r="E57" t="s">
+        <v>231</v>
+      </c>
+      <c r="F57" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6">
       <c r="A58" t="s">
         <v>176</v>
       </c>
@@ -2089,10 +2287,13 @@
         <v>400</v>
       </c>
       <c r="E58" t="s">
+        <v>234</v>
+      </c>
+      <c r="F58" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6">
       <c r="A59" t="s">
         <v>177</v>
       </c>
@@ -2106,10 +2307,13 @@
         <v>400</v>
       </c>
       <c r="E59" t="s">
+        <v>234</v>
+      </c>
+      <c r="F59" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6">
       <c r="A60" t="s">
         <v>178</v>
       </c>
@@ -2123,10 +2327,13 @@
         <v>15</v>
       </c>
       <c r="E60" t="s">
+        <v>234</v>
+      </c>
+      <c r="F60" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6">
       <c r="A61" t="s">
         <v>119</v>
       </c>
@@ -2140,10 +2347,13 @@
         <v>50</v>
       </c>
       <c r="E61" t="s">
+        <v>234</v>
+      </c>
+      <c r="F61" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6">
       <c r="A62" t="s">
         <v>179</v>
       </c>
@@ -2157,10 +2367,13 @@
         <v>50</v>
       </c>
       <c r="E62" t="s">
+        <v>234</v>
+      </c>
+      <c r="F62" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6">
       <c r="A63" t="s">
         <v>180</v>
       </c>
@@ -2174,10 +2387,13 @@
         <v>150</v>
       </c>
       <c r="E63" t="s">
+        <v>234</v>
+      </c>
+      <c r="F63" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6">
       <c r="A64" t="s">
         <v>181</v>
       </c>
@@ -2191,10 +2407,13 @@
         <v>300</v>
       </c>
       <c r="E64" t="s">
+        <v>234</v>
+      </c>
+      <c r="F64" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6">
       <c r="A65" t="s">
         <v>182</v>
       </c>
@@ -2208,10 +2427,13 @@
         <v>30</v>
       </c>
       <c r="E65" t="s">
+        <v>234</v>
+      </c>
+      <c r="F65" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6">
       <c r="A66" t="s">
         <v>183</v>
       </c>
@@ -2225,10 +2447,13 @@
         <v>15</v>
       </c>
       <c r="E66" t="s">
+        <v>234</v>
+      </c>
+      <c r="F66" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6">
       <c r="A67" t="s">
         <v>184</v>
       </c>
@@ -2242,10 +2467,13 @@
         <v>50</v>
       </c>
       <c r="E67" t="s">
+        <v>234</v>
+      </c>
+      <c r="F67" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6">
       <c r="A68" t="s">
         <v>185</v>
       </c>
@@ -2259,10 +2487,13 @@
         <v>0</v>
       </c>
       <c r="E68" t="s">
+        <v>233</v>
+      </c>
+      <c r="F68" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6">
       <c r="A69" t="s">
         <v>186</v>
       </c>
@@ -2276,10 +2507,13 @@
         <v>0</v>
       </c>
       <c r="E69" t="s">
+        <v>233</v>
+      </c>
+      <c r="F69" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6">
       <c r="A70" t="s">
         <v>187</v>
       </c>
@@ -2293,10 +2527,13 @@
         <v>0</v>
       </c>
       <c r="E70" t="s">
+        <v>233</v>
+      </c>
+      <c r="F70" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6">
       <c r="A71" t="s">
         <v>188</v>
       </c>
@@ -2310,10 +2547,13 @@
         <v>0</v>
       </c>
       <c r="E71" t="s">
+        <v>233</v>
+      </c>
+      <c r="F71" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6">
       <c r="A72" t="s">
         <v>189</v>
       </c>
@@ -2327,10 +2567,13 @@
         <v>100</v>
       </c>
       <c r="E72" t="s">
+        <v>234</v>
+      </c>
+      <c r="F72" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6">
       <c r="A73" t="s">
         <v>190</v>
       </c>
@@ -2344,10 +2587,13 @@
         <v>0</v>
       </c>
       <c r="E73" t="s">
+        <v>229</v>
+      </c>
+      <c r="F73" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6">
       <c r="A74" t="s">
         <v>191</v>
       </c>
@@ -2361,10 +2607,13 @@
         <v>100</v>
       </c>
       <c r="E74" t="s">
+        <v>234</v>
+      </c>
+      <c r="F74" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6">
       <c r="A75" t="s">
         <v>192</v>
       </c>
@@ -2378,10 +2627,13 @@
         <v>0</v>
       </c>
       <c r="E75" t="s">
+        <v>231</v>
+      </c>
+      <c r="F75" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6">
       <c r="A76" t="s">
         <v>193</v>
       </c>
@@ -2395,10 +2647,13 @@
         <v>0</v>
       </c>
       <c r="E76" t="s">
+        <v>232</v>
+      </c>
+      <c r="F76" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6">
       <c r="A77" t="s">
         <v>194</v>
       </c>
@@ -2412,10 +2667,13 @@
         <v>400</v>
       </c>
       <c r="E77" t="s">
+        <v>234</v>
+      </c>
+      <c r="F77" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6">
       <c r="A78" t="s">
         <v>195</v>
       </c>
@@ -2429,10 +2687,13 @@
         <v>0</v>
       </c>
       <c r="E78" t="s">
+        <v>235</v>
+      </c>
+      <c r="F78" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6">
       <c r="A79" t="s">
         <v>196</v>
       </c>
@@ -2446,10 +2707,13 @@
         <v>0</v>
       </c>
       <c r="E79" t="s">
+        <v>235</v>
+      </c>
+      <c r="F79" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6">
       <c r="A80" t="s">
         <v>197</v>
       </c>
@@ -2463,10 +2727,13 @@
         <v>0</v>
       </c>
       <c r="E80" t="s">
+        <v>235</v>
+      </c>
+      <c r="F80" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6">
       <c r="A81" t="s">
         <v>198</v>
       </c>
@@ -2480,10 +2747,13 @@
         <v>0</v>
       </c>
       <c r="E81" t="s">
+        <v>235</v>
+      </c>
+      <c r="F81" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6">
       <c r="A82" t="s">
         <v>199</v>
       </c>
@@ -2497,10 +2767,13 @@
         <v>0</v>
       </c>
       <c r="E82" t="s">
+        <v>235</v>
+      </c>
+      <c r="F82" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6">
       <c r="A83" t="s">
         <v>200</v>
       </c>
@@ -2514,10 +2787,13 @@
         <v>0</v>
       </c>
       <c r="E83" t="s">
+        <v>235</v>
+      </c>
+      <c r="F83" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6">
       <c r="A84" t="s">
         <v>201</v>
       </c>
@@ -2531,10 +2807,13 @@
         <v>0</v>
       </c>
       <c r="E84" t="s">
+        <v>235</v>
+      </c>
+      <c r="F84" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6">
       <c r="A85" t="s">
         <v>202</v>
       </c>
@@ -2548,10 +2827,13 @@
         <v>0</v>
       </c>
       <c r="E85" t="s">
+        <v>235</v>
+      </c>
+      <c r="F85" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6">
       <c r="A86" t="s">
         <v>203</v>
       </c>
@@ -2565,10 +2847,13 @@
         <v>0</v>
       </c>
       <c r="E86" t="s">
+        <v>235</v>
+      </c>
+      <c r="F86" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6">
       <c r="A87" t="s">
         <v>204</v>
       </c>
@@ -2582,10 +2867,13 @@
         <v>0</v>
       </c>
       <c r="E87" t="s">
+        <v>235</v>
+      </c>
+      <c r="F87" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6">
       <c r="A88" t="s">
         <v>205</v>
       </c>
@@ -2599,10 +2887,13 @@
         <v>0</v>
       </c>
       <c r="E88" t="s">
+        <v>235</v>
+      </c>
+      <c r="F88" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6">
       <c r="A89" t="s">
         <v>206</v>
       </c>
@@ -2616,10 +2907,13 @@
         <v>0</v>
       </c>
       <c r="E89" t="s">
+        <v>235</v>
+      </c>
+      <c r="F89" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6">
       <c r="A90" t="s">
         <v>207</v>
       </c>
@@ -2633,10 +2927,13 @@
         <v>0</v>
       </c>
       <c r="E90" t="s">
+        <v>235</v>
+      </c>
+      <c r="F90" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6">
       <c r="A91" t="s">
         <v>208</v>
       </c>
@@ -2650,10 +2947,13 @@
         <v>0</v>
       </c>
       <c r="E91" t="s">
+        <v>235</v>
+      </c>
+      <c r="F91" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6">
       <c r="A92" t="s">
         <v>209</v>
       </c>
@@ -2667,10 +2967,13 @@
         <v>0</v>
       </c>
       <c r="E92" t="s">
+        <v>235</v>
+      </c>
+      <c r="F92" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6">
       <c r="A93" t="s">
         <v>210</v>
       </c>
@@ -2684,10 +2987,13 @@
         <v>0</v>
       </c>
       <c r="E93" t="s">
+        <v>235</v>
+      </c>
+      <c r="F93" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6">
       <c r="A94" t="s">
         <v>211</v>
       </c>
@@ -2701,10 +3007,13 @@
         <v>0</v>
       </c>
       <c r="E94" t="s">
+        <v>235</v>
+      </c>
+      <c r="F94" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6">
       <c r="A95" t="s">
         <v>212</v>
       </c>
@@ -2718,10 +3027,13 @@
         <v>0</v>
       </c>
       <c r="E95" t="s">
+        <v>235</v>
+      </c>
+      <c r="F95" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6">
       <c r="A96" t="s">
         <v>213</v>
       </c>
@@ -2735,10 +3047,13 @@
         <v>0</v>
       </c>
       <c r="E96" t="s">
+        <v>235</v>
+      </c>
+      <c r="F96" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6">
       <c r="A97" t="s">
         <v>214</v>
       </c>
@@ -2752,10 +3067,13 @@
         <v>0</v>
       </c>
       <c r="E97" t="s">
+        <v>235</v>
+      </c>
+      <c r="F97" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6">
       <c r="A98" t="s">
         <v>215</v>
       </c>
@@ -2769,10 +3087,13 @@
         <v>0</v>
       </c>
       <c r="E98" t="s">
+        <v>235</v>
+      </c>
+      <c r="F98" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6">
       <c r="A99" t="s">
         <v>216</v>
       </c>
@@ -2786,10 +3107,13 @@
         <v>0</v>
       </c>
       <c r="E99" t="s">
+        <v>232</v>
+      </c>
+      <c r="F99" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6">
       <c r="A100" t="s">
         <v>217</v>
       </c>
@@ -2803,10 +3127,13 @@
         <v>0</v>
       </c>
       <c r="E100" t="s">
+        <v>231</v>
+      </c>
+      <c r="F100" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6">
       <c r="A101" t="s">
         <v>218</v>
       </c>
@@ -2820,10 +3147,13 @@
         <v>400</v>
       </c>
       <c r="E101" t="s">
+        <v>232</v>
+      </c>
+      <c r="F101" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6">
       <c r="A102" t="s">
         <v>219</v>
       </c>
@@ -2837,10 +3167,13 @@
         <v>400</v>
       </c>
       <c r="E102" t="s">
+        <v>232</v>
+      </c>
+      <c r="F102" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6">
       <c r="A103" t="s">
         <v>220</v>
       </c>
@@ -2854,10 +3187,13 @@
         <v>0</v>
       </c>
       <c r="E103" t="s">
+        <v>228</v>
+      </c>
+      <c r="F103" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6">
       <c r="A104" t="s">
         <v>221</v>
       </c>
@@ -2871,10 +3207,13 @@
         <v>0</v>
       </c>
       <c r="E104" t="s">
+        <v>228</v>
+      </c>
+      <c r="F104" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6">
       <c r="A105" t="s">
         <v>222</v>
       </c>
@@ -2888,10 +3227,13 @@
         <v>0</v>
       </c>
       <c r="E105" t="s">
+        <v>228</v>
+      </c>
+      <c r="F105" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6">
       <c r="A106" t="s">
         <v>223</v>
       </c>
@@ -2905,10 +3247,13 @@
         <v>0</v>
       </c>
       <c r="E106" t="s">
+        <v>228</v>
+      </c>
+      <c r="F106" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6">
       <c r="A107" t="s">
         <v>224</v>
       </c>
@@ -2922,10 +3267,13 @@
         <v>0</v>
       </c>
       <c r="E107" t="s">
+        <v>228</v>
+      </c>
+      <c r="F107" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6">
       <c r="A108" t="s">
         <v>225</v>
       </c>
@@ -2939,10 +3287,13 @@
         <v>0</v>
       </c>
       <c r="E108" t="s">
+        <v>228</v>
+      </c>
+      <c r="F108" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6">
       <c r="A109" t="s">
         <v>226</v>
       </c>
@@ -2956,12 +3307,15 @@
         <v>0</v>
       </c>
       <c r="E109" t="s">
+        <v>228</v>
+      </c>
+      <c r="F109" t="s">
         <v>65</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E109" xr:uid="{243C1198-9050-4D31-9385-CFB2A1D9CA84}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E109">
+  <autoFilter ref="A1:F109">
+    <sortState ref="A2:E109">
       <sortCondition ref="A1:A109"/>
     </sortState>
   </autoFilter>

</xml_diff>